<commit_message>
next generation of this solution
</commit_message>
<xml_diff>
--- a/Attune_Estate_2022_Bookings.xlsx
+++ b/Attune_Estate_2022_Bookings.xlsx
@@ -70,7 +70,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment shrinkToFit="1"/>
@@ -86,6 +86,9 @@
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +467,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -553,7 +557,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G2" s="3" t="n"/>
+      <c r="G2" s="6" t="n"/>
       <c r="H2" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -565,7 +569,7 @@
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
     </row>
@@ -592,7 +596,7 @@
           <t>Res. - Renter</t>
         </is>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="6" t="n">
         <v>5700</v>
       </c>
       <c r="H3" s="5" t="inlineStr">
@@ -606,7 +610,7 @@
         </is>
       </c>
       <c r="J3" s="5" t="n"/>
-      <c r="K3" s="3" t="n"/>
+      <c r="K3" s="4" t="n"/>
       <c r="L3" s="4" t="n"/>
       <c r="M3" s="3" t="n"/>
     </row>
@@ -633,7 +637,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G4" s="3" t="n"/>
+      <c r="G4" s="6" t="n"/>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -645,7 +649,7 @@
         </is>
       </c>
       <c r="J4" s="5" t="n"/>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="4" t="n"/>
       <c r="L4" s="4" t="n"/>
       <c r="M4" s="3" t="n"/>
     </row>
@@ -672,7 +676,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G5" s="3" t="n"/>
+      <c r="G5" s="6" t="n"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -684,7 +688,7 @@
         </is>
       </c>
       <c r="J5" s="5" t="n"/>
-      <c r="K5" s="3" t="n"/>
+      <c r="K5" s="4" t="n"/>
       <c r="L5" s="4" t="n"/>
       <c r="M5" s="3" t="n"/>
     </row>
@@ -711,7 +715,7 @@
           <t>Res. - Renter</t>
         </is>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="6" t="n">
         <v>5700</v>
       </c>
       <c r="H6" s="5" t="inlineStr">
@@ -725,7 +729,7 @@
         </is>
       </c>
       <c r="J6" s="5" t="n"/>
-      <c r="K6" s="3" t="n"/>
+      <c r="K6" s="4" t="n"/>
       <c r="L6" s="4" t="n"/>
       <c r="M6" s="3" t="n"/>
     </row>
@@ -752,7 +756,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G7" s="3" t="n"/>
+      <c r="G7" s="6" t="n"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -764,7 +768,7 @@
         </is>
       </c>
       <c r="J7" s="5" t="n"/>
-      <c r="K7" s="3" t="n"/>
+      <c r="K7" s="4" t="n"/>
       <c r="L7" s="4" t="n"/>
       <c r="M7" s="3" t="n"/>
     </row>
@@ -772,7 +776,7 @@
       <c r="A8" s="3" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>MLH-00010</t>
+          <t>HLD-22490</t>
         </is>
       </c>
       <c r="C8" s="4" t="n">
@@ -789,7 +793,7 @@
           <t>Hold-Deep Clean</t>
         </is>
       </c>
-      <c r="G8" s="3" t="n"/>
+      <c r="G8" s="6" t="n"/>
       <c r="H8" s="5" t="inlineStr">
         <is>
           <t>MS</t>
@@ -801,7 +805,7 @@
         </is>
       </c>
       <c r="J8" s="5" t="n"/>
-      <c r="K8" s="3" t="n"/>
+      <c r="K8" s="4" t="n"/>
       <c r="L8" s="4" t="n"/>
       <c r="M8" s="3" t="n"/>
     </row>
@@ -828,7 +832,7 @@
           <t>Hold - Owner</t>
         </is>
       </c>
-      <c r="G9" s="3" t="n"/>
+      <c r="G9" s="6" t="n"/>
       <c r="H9" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -840,7 +844,7 @@
         </is>
       </c>
       <c r="J9" s="5" t="n"/>
-      <c r="K9" s="3" t="n"/>
+      <c r="K9" s="4" t="n"/>
       <c r="L9" s="4" t="n"/>
       <c r="M9" s="3" t="n"/>
     </row>
@@ -865,7 +869,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G10" s="3" t="n"/>
+      <c r="G10" s="6" t="n"/>
       <c r="H10" s="5" t="inlineStr">
         <is>
           <t>Marthas Cleaning</t>
@@ -881,7 +885,7 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K10" s="3" t="n"/>
+      <c r="K10" s="4" t="n"/>
       <c r="L10" s="4" t="n"/>
       <c r="M10" s="3" t="n"/>
     </row>
@@ -906,7 +910,7 @@
           <t>Res. - Renter</t>
         </is>
       </c>
-      <c r="G11" s="3" t="n">
+      <c r="G11" s="6" t="n">
         <v>5881</v>
       </c>
       <c r="H11" s="5" t="inlineStr">
@@ -924,7 +928,7 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K11" s="3" t="n"/>
+      <c r="K11" s="4" t="n"/>
       <c r="L11" s="4" t="n"/>
       <c r="M11" s="3" t="n"/>
     </row>
@@ -949,7 +953,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G12" s="3" t="n"/>
+      <c r="G12" s="6" t="n"/>
       <c r="H12" s="5" t="inlineStr">
         <is>
           <t>MS</t>
@@ -965,7 +969,7 @@
           <t>N</t>
         </is>
       </c>
-      <c r="K12" s="3" t="n"/>
+      <c r="K12" s="4" t="n"/>
       <c r="L12" s="4" t="n"/>
       <c r="M12" s="3" t="n"/>
     </row>
@@ -992,7 +996,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G13" s="3" t="n"/>
+      <c r="G13" s="6" t="n"/>
       <c r="H13" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1004,7 +1008,7 @@
         </is>
       </c>
       <c r="J13" s="5" t="n"/>
-      <c r="K13" s="3" t="n"/>
+      <c r="K13" s="4" t="n"/>
       <c r="L13" s="4" t="n"/>
       <c r="M13" s="3" t="n"/>
     </row>
@@ -1031,7 +1035,7 @@
           <t>Res. - Renter</t>
         </is>
       </c>
-      <c r="G14" s="3" t="n">
+      <c r="G14" s="6" t="n">
         <v>5700</v>
       </c>
       <c r="H14" s="5" t="inlineStr">
@@ -1045,7 +1049,7 @@
         </is>
       </c>
       <c r="J14" s="5" t="n"/>
-      <c r="K14" s="3" t="n"/>
+      <c r="K14" s="4" t="n"/>
       <c r="L14" s="4" t="n"/>
       <c r="M14" s="3" t="n"/>
     </row>
@@ -1053,7 +1057,7 @@
       <c r="A15" s="3" t="n"/>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>HLD-22511</t>
+          <t>CLN-00030</t>
         </is>
       </c>
       <c r="C15" s="4" t="n">
@@ -1072,7 +1076,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G15" s="3" t="n"/>
+      <c r="G15" s="6" t="n"/>
       <c r="H15" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1084,7 +1088,7 @@
         </is>
       </c>
       <c r="J15" s="5" t="n"/>
-      <c r="K15" s="3" t="n"/>
+      <c r="K15" s="4" t="n"/>
       <c r="L15" s="4" t="n"/>
       <c r="M15" s="3" t="n"/>
     </row>
@@ -1092,66 +1096,66 @@
       <c r="A16" s="3" t="n"/>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>MLS-00040</t>
+          <t>CLN-00100</t>
         </is>
       </c>
       <c r="C16" s="4" t="n">
         <v>44629</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>44633</v>
+        <v>44629</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>Hold - Renter</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="n"/>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G16" s="6" t="n"/>
       <c r="H16" s="5" t="inlineStr">
         <is>
+          <t>MS-Add</t>
+        </is>
+      </c>
+      <c r="I16" s="5" t="inlineStr">
+        <is>
           <t>MS</t>
         </is>
       </c>
-      <c r="I16" s="5" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
       <c r="J16" s="5" t="n"/>
-      <c r="K16" s="3" t="n"/>
-      <c r="L16" s="4" t="n">
-        <v>44593</v>
-      </c>
+      <c r="K16" s="4" t="n"/>
+      <c r="L16" s="4" t="n"/>
       <c r="M16" s="3" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="3" t="n"/>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>CLN-00060</t>
+          <t>MLS-00020</t>
         </is>
       </c>
       <c r="C17" s="4" t="n">
-        <v>44634</v>
+        <v>44630</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>44634</v>
+        <v>44633</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
-          <t>Hold - Clean</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>5175</v>
+      </c>
       <c r="H17" s="5" t="inlineStr">
         <is>
-          <t>MS-Add</t>
+          <t>Airbnb</t>
         </is>
       </c>
       <c r="I17" s="5" t="inlineStr">
@@ -1160,7 +1164,7 @@
         </is>
       </c>
       <c r="J17" s="5" t="n"/>
-      <c r="K17" s="3" t="n"/>
+      <c r="K17" s="4" t="n"/>
       <c r="L17" s="4" t="n"/>
       <c r="M17" s="3" t="n"/>
     </row>
@@ -1168,36 +1172,38 @@
       <c r="A18" s="3" t="n"/>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>CLN-00070</t>
+          <t>CLN-00040</t>
         </is>
       </c>
       <c r="C18" s="4" t="n">
-        <v>44643</v>
+        <v>44634</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>44643</v>
-      </c>
-      <c r="E18" s="5" t="n">
-        <v>1</v>
+        <v>44634</v>
+      </c>
+      <c r="E18" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G18" s="3" t="n"/>
+      <c r="G18" s="6" t="n"/>
       <c r="H18" s="5" t="inlineStr">
         <is>
-          <t>MS-Add</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="I18" s="5" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="J18" s="5" t="n"/>
-      <c r="K18" s="3" t="n"/>
+      <c r="K18" s="4" t="n"/>
       <c r="L18" s="4" t="n"/>
       <c r="M18" s="3" t="n"/>
     </row>
@@ -1205,29 +1211,27 @@
       <c r="A19" s="3" t="n"/>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>MLS-00050</t>
+          <t>CLN-00110</t>
         </is>
       </c>
       <c r="C19" s="4" t="n">
-        <v>44644</v>
+        <v>44643</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>44647</v>
+        <v>44643</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G19" s="3" t="n">
-        <v>5684.28</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G19" s="6" t="n"/>
       <c r="H19" s="5" t="inlineStr">
         <is>
-          <t>Airbnb</t>
+          <t>MS-Add</t>
         </is>
       </c>
       <c r="I19" s="5" t="inlineStr">
@@ -1236,7 +1240,7 @@
         </is>
       </c>
       <c r="J19" s="5" t="n"/>
-      <c r="K19" s="3" t="n"/>
+      <c r="K19" s="4" t="n"/>
       <c r="L19" s="4" t="n"/>
       <c r="M19" s="3" t="n"/>
     </row>
@@ -1244,36 +1248,38 @@
       <c r="A20" s="3" t="n"/>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>OWN-00010</t>
+          <t>MLS-00030</t>
         </is>
       </c>
       <c r="C20" s="4" t="n">
+        <v>44644</v>
+      </c>
+      <c r="D20" s="4" t="n">
         <v>44647</v>
       </c>
-      <c r="D20" s="4" t="n">
-        <v>44649</v>
-      </c>
       <c r="E20" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
-          <t>Res.-Owner</t>
-        </is>
-      </c>
-      <c r="G20" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>5684.28</v>
+      </c>
       <c r="H20" s="5" t="inlineStr">
         <is>
+          <t>Airbnb</t>
+        </is>
+      </c>
+      <c r="I20" s="5" t="inlineStr">
+        <is>
           <t>MS</t>
         </is>
       </c>
-      <c r="I20" s="5" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
       <c r="J20" s="5" t="n"/>
-      <c r="K20" s="3" t="n"/>
+      <c r="K20" s="4" t="n"/>
       <c r="L20" s="4" t="n"/>
       <c r="M20" s="3" t="n"/>
     </row>
@@ -1281,14 +1287,14 @@
       <c r="A21" s="3" t="n"/>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>CLN-00080</t>
+          <t>CLN-00050</t>
         </is>
       </c>
       <c r="C21" s="4" t="n">
-        <v>44650</v>
+        <v>44647</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>44650</v>
+        <v>44647</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>1</v>
@@ -1298,10 +1304,10 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G21" s="3" t="n"/>
+      <c r="G21" s="6" t="n"/>
       <c r="H21" s="5" t="inlineStr">
         <is>
-          <t>MS-Add</t>
+          <t>Marthas</t>
         </is>
       </c>
       <c r="I21" s="5" t="inlineStr">
@@ -1310,7 +1316,7 @@
         </is>
       </c>
       <c r="J21" s="5" t="n"/>
-      <c r="K21" s="3" t="n"/>
+      <c r="K21" s="4" t="n"/>
       <c r="L21" s="4" t="n"/>
       <c r="M21" s="3" t="n"/>
     </row>
@@ -1318,38 +1324,36 @@
       <c r="A22" s="3" t="n"/>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>HLD-22639</t>
+          <t>OWN-00010</t>
         </is>
       </c>
       <c r="C22" s="4" t="n">
-        <v>44659</v>
+        <v>44647</v>
       </c>
       <c r="D22" s="4" t="n">
-        <v>44659</v>
-      </c>
-      <c r="E22" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+        <v>44649</v>
+      </c>
+      <c r="E22" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
-          <t>Hold - Clean</t>
-        </is>
-      </c>
-      <c r="G22" s="3" t="n"/>
+          <t>Res.-Owner</t>
+        </is>
+      </c>
+      <c r="G22" s="6" t="n"/>
       <c r="H22" s="5" t="inlineStr">
         <is>
-          <t>BP</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="I22" s="5" t="inlineStr">
         <is>
-          <t>BP</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="J22" s="5" t="n"/>
-      <c r="K22" s="3" t="n"/>
+      <c r="K22" s="4" t="n"/>
       <c r="L22" s="4" t="n"/>
       <c r="M22" s="3" t="n"/>
     </row>
@@ -1357,40 +1361,36 @@
       <c r="A23" s="3" t="n"/>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>BKG-11586</t>
+          <t>CLN-00060</t>
         </is>
       </c>
       <c r="C23" s="4" t="n">
-        <v>44660</v>
+        <v>44650</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>44664</v>
-      </c>
-      <c r="E23" s="5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+        <v>44650</v>
+      </c>
+      <c r="E23" s="5" t="n">
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G23" s="3" t="n">
-        <v>9875</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G23" s="6" t="n"/>
       <c r="H23" s="5" t="inlineStr">
         <is>
-          <t>BP</t>
+          <t>Marthas</t>
         </is>
       </c>
       <c r="I23" s="5" t="inlineStr">
         <is>
-          <t>BP</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="J23" s="5" t="n"/>
-      <c r="K23" s="3" t="n"/>
+      <c r="K23" s="4" t="n"/>
       <c r="L23" s="4" t="n"/>
       <c r="M23" s="3" t="n"/>
     </row>
@@ -1398,14 +1398,14 @@
       <c r="A24" s="3" t="n"/>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>HLD-22640</t>
+          <t>HLD-22639</t>
         </is>
       </c>
       <c r="C24" s="4" t="n">
-        <v>44665</v>
+        <v>44659</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>44665</v>
+        <v>44659</v>
       </c>
       <c r="E24" s="5" t="inlineStr">
         <is>
@@ -1417,7 +1417,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G24" s="3" t="n"/>
+      <c r="G24" s="6" t="n"/>
       <c r="H24" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="J24" s="5" t="n"/>
-      <c r="K24" s="3" t="n"/>
+      <c r="K24" s="4" t="n"/>
       <c r="L24" s="4" t="n"/>
       <c r="M24" s="3" t="n"/>
     </row>
@@ -1437,26 +1437,28 @@
       <c r="A25" s="3" t="n"/>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>HLD-22429</t>
+          <t>BKG-11586</t>
         </is>
       </c>
       <c r="C25" s="4" t="n">
-        <v>44669</v>
+        <v>44660</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>44669</v>
+        <v>44664</v>
       </c>
       <c r="E25" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>Hold - Clean</t>
-        </is>
-      </c>
-      <c r="G25" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G25" s="6" t="n">
+        <v>9875</v>
+      </c>
       <c r="H25" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1468,7 +1470,7 @@
         </is>
       </c>
       <c r="J25" s="5" t="n"/>
-      <c r="K25" s="3" t="n"/>
+      <c r="K25" s="4" t="n"/>
       <c r="L25" s="4" t="n"/>
       <c r="M25" s="3" t="n"/>
     </row>
@@ -1476,28 +1478,26 @@
       <c r="A26" s="3" t="n"/>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>BKG-11520</t>
+          <t>HLD-22640</t>
         </is>
       </c>
       <c r="C26" s="4" t="n">
-        <v>44670</v>
+        <v>44665</v>
       </c>
       <c r="D26" s="4" t="n">
-        <v>44674</v>
+        <v>44665</v>
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G26" s="3" t="n">
-        <v>9875</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G26" s="6" t="n"/>
       <c r="H26" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1509,7 +1509,7 @@
         </is>
       </c>
       <c r="J26" s="5" t="n"/>
-      <c r="K26" s="3" t="n"/>
+      <c r="K26" s="4" t="n"/>
       <c r="L26" s="4" t="n"/>
       <c r="M26" s="3" t="n"/>
     </row>
@@ -1517,14 +1517,14 @@
       <c r="A27" s="3" t="n"/>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>HLD-22430</t>
+          <t>HLD-22429</t>
         </is>
       </c>
       <c r="C27" s="4" t="n">
-        <v>44675</v>
+        <v>44669</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>44675</v>
+        <v>44669</v>
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
@@ -1536,7 +1536,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G27" s="3" t="n"/>
+      <c r="G27" s="6" t="n"/>
       <c r="H27" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1548,7 +1548,7 @@
         </is>
       </c>
       <c r="J27" s="5" t="n"/>
-      <c r="K27" s="3" t="n"/>
+      <c r="K27" s="4" t="n"/>
       <c r="L27" s="4" t="n"/>
       <c r="M27" s="3" t="n"/>
     </row>
@@ -1556,26 +1556,28 @@
       <c r="A28" s="3" t="n"/>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>HLD-22650</t>
+          <t>BKG-11520</t>
         </is>
       </c>
       <c r="C28" s="4" t="n">
-        <v>44677</v>
+        <v>44670</v>
       </c>
       <c r="D28" s="4" t="n">
-        <v>44677</v>
+        <v>44674</v>
       </c>
       <c r="E28" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>Hold - Clean</t>
-        </is>
-      </c>
-      <c r="G28" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G28" s="6" t="n">
+        <v>9875</v>
+      </c>
       <c r="H28" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1587,7 +1589,7 @@
         </is>
       </c>
       <c r="J28" s="5" t="n"/>
-      <c r="K28" s="3" t="n"/>
+      <c r="K28" s="4" t="n"/>
       <c r="L28" s="4" t="n"/>
       <c r="M28" s="3" t="n"/>
     </row>
@@ -1595,28 +1597,26 @@
       <c r="A29" s="3" t="n"/>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>BKG-11588</t>
+          <t>HLD-22430</t>
         </is>
       </c>
       <c r="C29" s="4" t="n">
-        <v>44678</v>
+        <v>44675</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>44684</v>
+        <v>44675</v>
       </c>
       <c r="E29" s="5" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G29" s="3" t="n">
-        <v>13825</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G29" s="6" t="n"/>
       <c r="H29" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1628,7 +1628,7 @@
         </is>
       </c>
       <c r="J29" s="5" t="n"/>
-      <c r="K29" s="3" t="n"/>
+      <c r="K29" s="4" t="n"/>
       <c r="L29" s="4" t="n"/>
       <c r="M29" s="3" t="n"/>
     </row>
@@ -1636,14 +1636,14 @@
       <c r="A30" s="3" t="n"/>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>HLD-22651</t>
+          <t>HLD-22650</t>
         </is>
       </c>
       <c r="C30" s="4" t="n">
-        <v>44685</v>
+        <v>44677</v>
       </c>
       <c r="D30" s="4" t="n">
-        <v>44685</v>
+        <v>44677</v>
       </c>
       <c r="E30" s="5" t="inlineStr">
         <is>
@@ -1655,7 +1655,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G30" s="3" t="n"/>
+      <c r="G30" s="6" t="n"/>
       <c r="H30" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1667,7 +1667,7 @@
         </is>
       </c>
       <c r="J30" s="5" t="n"/>
-      <c r="K30" s="3" t="n"/>
+      <c r="K30" s="4" t="n"/>
       <c r="L30" s="4" t="n"/>
       <c r="M30" s="3" t="n"/>
     </row>
@@ -1675,26 +1675,28 @@
       <c r="A31" s="3" t="n"/>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>HLD-22529</t>
+          <t>BKG-11588</t>
         </is>
       </c>
       <c r="C31" s="4" t="n">
-        <v>44691</v>
+        <v>44678</v>
       </c>
       <c r="D31" s="4" t="n">
-        <v>44691</v>
+        <v>44684</v>
       </c>
       <c r="E31" s="5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
-          <t>Hold - Clean</t>
-        </is>
-      </c>
-      <c r="G31" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>13825</v>
+      </c>
       <c r="H31" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1706,7 +1708,7 @@
         </is>
       </c>
       <c r="J31" s="5" t="n"/>
-      <c r="K31" s="3" t="n"/>
+      <c r="K31" s="4" t="n"/>
       <c r="L31" s="4" t="n"/>
       <c r="M31" s="3" t="n"/>
     </row>
@@ -1714,28 +1716,26 @@
       <c r="A32" s="3" t="n"/>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>BKG-11547</t>
+          <t>HLD-22651</t>
         </is>
       </c>
       <c r="C32" s="4" t="n">
-        <v>44692</v>
+        <v>44685</v>
       </c>
       <c r="D32" s="4" t="n">
-        <v>44695</v>
+        <v>44685</v>
       </c>
       <c r="E32" s="5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G32" s="3" t="n">
-        <v>7900</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G32" s="6" t="n"/>
       <c r="H32" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="J32" s="5" t="n"/>
-      <c r="K32" s="3" t="n"/>
+      <c r="K32" s="4" t="n"/>
       <c r="L32" s="4" t="n"/>
       <c r="M32" s="3" t="n"/>
     </row>
@@ -1755,14 +1755,14 @@
       <c r="A33" s="3" t="n"/>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>HLD-22530</t>
+          <t>HLD-22529</t>
         </is>
       </c>
       <c r="C33" s="4" t="n">
-        <v>44696</v>
+        <v>44691</v>
       </c>
       <c r="D33" s="4" t="n">
-        <v>44696</v>
+        <v>44691</v>
       </c>
       <c r="E33" s="5" t="inlineStr">
         <is>
@@ -1774,7 +1774,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G33" s="3" t="n"/>
+      <c r="G33" s="6" t="n"/>
       <c r="H33" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -1786,7 +1786,7 @@
         </is>
       </c>
       <c r="J33" s="5" t="n"/>
-      <c r="K33" s="3" t="n"/>
+      <c r="K33" s="4" t="n"/>
       <c r="L33" s="4" t="n"/>
       <c r="M33" s="3" t="n"/>
     </row>
@@ -1794,38 +1794,40 @@
       <c r="A34" s="3" t="n"/>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>MLS-00030</t>
+          <t>BKG-11547</t>
         </is>
       </c>
       <c r="C34" s="4" t="n">
-        <v>44700</v>
+        <v>44692</v>
       </c>
       <c r="D34" s="4" t="n">
-        <v>44705</v>
-      </c>
-      <c r="E34" s="5" t="n">
-        <v>5</v>
+        <v>44695</v>
+      </c>
+      <c r="E34" s="5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
           <t>Res. - Renter</t>
         </is>
       </c>
-      <c r="G34" s="3" t="n">
-        <v>11678.8</v>
+      <c r="G34" s="6" t="n">
+        <v>7900</v>
       </c>
       <c r="H34" s="5" t="inlineStr">
         <is>
-          <t>AirBnb</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="I34" s="5" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="J34" s="5" t="n"/>
-      <c r="K34" s="3" t="n"/>
+      <c r="K34" s="4" t="n"/>
       <c r="L34" s="4" t="n"/>
       <c r="M34" s="3" t="n"/>
     </row>
@@ -1833,36 +1835,38 @@
       <c r="A35" s="3" t="n"/>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>CLN-00030</t>
+          <t>CLN-00070</t>
         </is>
       </c>
       <c r="C35" s="4" t="n">
-        <v>44706</v>
+        <v>44696</v>
       </c>
       <c r="D35" s="4" t="n">
-        <v>44706</v>
-      </c>
-      <c r="E35" s="5" t="n">
-        <v>1</v>
+        <v>44696</v>
+      </c>
+      <c r="E35" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G35" s="3" t="n"/>
+      <c r="G35" s="6" t="n"/>
       <c r="H35" s="5" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="I35" s="5" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="J35" s="5" t="n"/>
-      <c r="K35" s="3" t="n"/>
+      <c r="K35" s="4" t="n"/>
       <c r="L35" s="4" t="n"/>
       <c r="M35" s="3" t="n"/>
     </row>
@@ -1870,29 +1874,27 @@
       <c r="A36" s="3" t="n"/>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>MLS-00020</t>
+          <t>CLN-00120</t>
         </is>
       </c>
       <c r="C36" s="4" t="n">
-        <v>44707</v>
+        <v>44699</v>
       </c>
       <c r="D36" s="4" t="n">
-        <v>44712</v>
+        <v>44699</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G36" s="3" t="n">
-        <v>5881</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G36" s="6" t="n"/>
       <c r="H36" s="5" t="inlineStr">
         <is>
-          <t>AirBnb</t>
+          <t>MS-Add</t>
         </is>
       </c>
       <c r="I36" s="5" t="inlineStr">
@@ -1901,7 +1903,7 @@
         </is>
       </c>
       <c r="J36" s="5" t="n"/>
-      <c r="K36" s="3" t="n"/>
+      <c r="K36" s="4" t="n"/>
       <c r="L36" s="4" t="n"/>
       <c r="M36" s="3" t="n"/>
     </row>
@@ -1909,29 +1911,29 @@
       <c r="A37" s="3" t="n"/>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>MLS-00060</t>
+          <t>MLS-00040</t>
         </is>
       </c>
       <c r="C37" s="4" t="n">
-        <v>44713</v>
+        <v>44700</v>
       </c>
       <c r="D37" s="4" t="n">
-        <v>44742</v>
-      </c>
-      <c r="E37" s="5" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+        <v>44705</v>
+      </c>
+      <c r="E37" s="5" t="n">
+        <v>5</v>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>Hold - Renter</t>
-        </is>
-      </c>
-      <c r="G37" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G37" s="6" t="n">
+        <v>11678.8</v>
+      </c>
       <c r="H37" s="5" t="inlineStr">
         <is>
-          <t>WineClub</t>
+          <t>AirBnb</t>
         </is>
       </c>
       <c r="I37" s="5" t="inlineStr">
@@ -1940,7 +1942,7 @@
         </is>
       </c>
       <c r="J37" s="5" t="n"/>
-      <c r="K37" s="3" t="n"/>
+      <c r="K37" s="4" t="n"/>
       <c r="L37" s="4" t="n"/>
       <c r="M37" s="3" t="n"/>
     </row>
@@ -1948,14 +1950,14 @@
       <c r="A38" s="3" t="n"/>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>CLN-00040</t>
+          <t>CLN-00080</t>
         </is>
       </c>
       <c r="C38" s="4" t="n">
-        <v>44743</v>
+        <v>44706</v>
       </c>
       <c r="D38" s="4" t="n">
-        <v>44743</v>
+        <v>44706</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>1</v>
@@ -1965,7 +1967,7 @@
           <t>Hold - Clean</t>
         </is>
       </c>
-      <c r="G38" s="3" t="n"/>
+      <c r="G38" s="6" t="n"/>
       <c r="H38" s="5" t="inlineStr">
         <is>
           <t>MS</t>
@@ -1977,7 +1979,7 @@
         </is>
       </c>
       <c r="J38" s="5" t="n"/>
-      <c r="K38" s="3" t="n"/>
+      <c r="K38" s="4" t="n"/>
       <c r="L38" s="4" t="n"/>
       <c r="M38" s="3" t="n"/>
     </row>
@@ -1985,38 +1987,38 @@
       <c r="A39" s="3" t="n"/>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>BKG-11547</t>
+          <t>MLS-00050</t>
         </is>
       </c>
       <c r="C39" s="4" t="n">
-        <v>44775</v>
+        <v>44707</v>
       </c>
       <c r="D39" s="4" t="n">
-        <v>44780</v>
+        <v>44712</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
           <t>Res. - Renter</t>
         </is>
       </c>
-      <c r="G39" s="3" t="n">
-        <v>12500</v>
+      <c r="G39" s="6" t="n">
+        <v>5881</v>
       </c>
       <c r="H39" s="5" t="inlineStr">
         <is>
-          <t>BP</t>
+          <t>AirBnb</t>
         </is>
       </c>
       <c r="I39" s="5" t="inlineStr">
         <is>
-          <t>BP</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="J39" s="5" t="n"/>
-      <c r="K39" s="3" t="n"/>
+      <c r="K39" s="4" t="n"/>
       <c r="L39" s="4" t="n"/>
       <c r="M39" s="3" t="n"/>
     </row>
@@ -2024,26 +2026,26 @@
       <c r="A40" s="3" t="n"/>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>HLD-22617</t>
+          <t>HLD-22839</t>
         </is>
       </c>
       <c r="C40" s="4" t="n">
-        <v>44919</v>
+        <v>44713</v>
       </c>
       <c r="D40" s="4" t="n">
-        <v>44930</v>
+        <v>44742</v>
       </c>
       <c r="E40" s="5" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>30</t>
         </is>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
-          <t>Hold - Other</t>
-        </is>
-      </c>
-      <c r="G40" s="3" t="n"/>
+          <t>Hold - Owner</t>
+        </is>
+      </c>
+      <c r="G40" s="6" t="n"/>
       <c r="H40" s="5" t="inlineStr">
         <is>
           <t>BP</t>
@@ -2055,9 +2057,239 @@
         </is>
       </c>
       <c r="J40" s="5" t="n"/>
-      <c r="K40" s="3" t="n"/>
+      <c r="K40" s="4" t="n"/>
       <c r="L40" s="4" t="n"/>
       <c r="M40" s="3" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="n"/>
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>CLN-00090</t>
+        </is>
+      </c>
+      <c r="C41" s="4" t="n">
+        <v>44713</v>
+      </c>
+      <c r="D41" s="4" t="n">
+        <v>44713</v>
+      </c>
+      <c r="E41" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G41" s="6" t="n"/>
+      <c r="H41" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="I41" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J41" s="5" t="n"/>
+      <c r="K41" s="4" t="n"/>
+      <c r="L41" s="4" t="n"/>
+      <c r="M41" s="3" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="n"/>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>BKG-11547</t>
+        </is>
+      </c>
+      <c r="C42" s="4" t="n">
+        <v>44775</v>
+      </c>
+      <c r="D42" s="4" t="n">
+        <v>44780</v>
+      </c>
+      <c r="E42" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G42" s="6" t="n">
+        <v>12500</v>
+      </c>
+      <c r="H42" s="5" t="inlineStr">
+        <is>
+          <t>BP</t>
+        </is>
+      </c>
+      <c r="I42" s="5" t="inlineStr">
+        <is>
+          <t>BP</t>
+        </is>
+      </c>
+      <c r="J42" s="5" t="n"/>
+      <c r="K42" s="4" t="n"/>
+      <c r="L42" s="4" t="n"/>
+      <c r="M42" s="3" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="n"/>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>CLN-00130</t>
+        </is>
+      </c>
+      <c r="C43" s="4" t="n">
+        <v>44805</v>
+      </c>
+      <c r="D43" s="4" t="n">
+        <v>44805</v>
+      </c>
+      <c r="E43" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G43" s="6" t="n"/>
+      <c r="H43" s="5" t="inlineStr">
+        <is>
+          <t>MS-Add</t>
+        </is>
+      </c>
+      <c r="I43" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J43" s="5" t="n"/>
+      <c r="K43" s="4" t="n"/>
+      <c r="L43" s="4" t="n"/>
+      <c r="M43" s="3" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="n"/>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>MLS-00060</t>
+        </is>
+      </c>
+      <c r="C44" s="4" t="n">
+        <v>44806</v>
+      </c>
+      <c r="D44" s="4" t="n">
+        <v>44808</v>
+      </c>
+      <c r="E44" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G44" s="6" t="n">
+        <v>6954</v>
+      </c>
+      <c r="H44" s="5" t="inlineStr">
+        <is>
+          <t>Airbnb</t>
+        </is>
+      </c>
+      <c r="I44" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J44" s="5" t="n"/>
+      <c r="K44" s="4" t="n">
+        <v>44595</v>
+      </c>
+      <c r="L44" s="4" t="n"/>
+      <c r="M44" s="3" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="n"/>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>CLN-00140</t>
+        </is>
+      </c>
+      <c r="C45" s="4" t="n">
+        <v>44809</v>
+      </c>
+      <c r="D45" s="4" t="n">
+        <v>44809</v>
+      </c>
+      <c r="E45" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G45" s="6" t="n"/>
+      <c r="H45" s="5" t="inlineStr">
+        <is>
+          <t>MS-Add</t>
+        </is>
+      </c>
+      <c r="I45" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J45" s="5" t="n"/>
+      <c r="K45" s="4" t="n"/>
+      <c r="L45" s="4" t="n"/>
+      <c r="M45" s="3" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="n"/>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>HLD-22617</t>
+        </is>
+      </c>
+      <c r="C46" s="4" t="n">
+        <v>44919</v>
+      </c>
+      <c r="D46" s="4" t="n">
+        <v>44930</v>
+      </c>
+      <c r="E46" s="5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>Hold - Other</t>
+        </is>
+      </c>
+      <c r="G46" s="6" t="n"/>
+      <c r="H46" s="5" t="inlineStr">
+        <is>
+          <t>BP</t>
+        </is>
+      </c>
+      <c r="I46" s="5" t="inlineStr">
+        <is>
+          <t>BP</t>
+        </is>
+      </c>
+      <c r="J46" s="5" t="n"/>
+      <c r="K46" s="4" t="n"/>
+      <c r="L46" s="4" t="n"/>
+      <c r="M46" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2070,7 +2302,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2082,6 +2314,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -2147,6 +2380,121 @@
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>CLN-00130</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>44805</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44805</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="5" t="inlineStr">
+        <is>
+          <t>MS-Add</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J2" s="5" t="n"/>
+      <c r="K2" s="4" t="n"/>
+      <c r="L2" s="4" t="n"/>
+      <c r="M2" s="3" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>MLS-00060</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>44806</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44808</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>6954</v>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>Airbnb</t>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="n"/>
+      <c r="K3" s="4" t="n">
+        <v>44595</v>
+      </c>
+      <c r="L3" s="4" t="n"/>
+      <c r="M3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>CLN-00140</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>44809</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44809</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="n"/>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>MS-Add</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="n"/>
+      <c r="K4" s="4" t="n"/>
+      <c r="L4" s="4" t="n"/>
+      <c r="M4" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2171,6 +2519,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -2260,6 +2609,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -2349,6 +2699,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -2450,7 +2801,7 @@
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
     </row>
@@ -2477,6 +2828,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -2578,7 +2930,7 @@
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
     </row>
@@ -2619,7 +2971,7 @@
         </is>
       </c>
       <c r="J3" s="5" t="n"/>
-      <c r="K3" s="3" t="n"/>
+      <c r="K3" s="4" t="n"/>
       <c r="L3" s="4" t="n"/>
       <c r="M3" s="3" t="n"/>
     </row>
@@ -2658,7 +3010,7 @@
         </is>
       </c>
       <c r="J4" s="5" t="n"/>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="4" t="n"/>
       <c r="L4" s="4" t="n"/>
       <c r="M4" s="3" t="n"/>
     </row>
@@ -2697,7 +3049,7 @@
         </is>
       </c>
       <c r="J5" s="5" t="n"/>
-      <c r="K5" s="3" t="n"/>
+      <c r="K5" s="4" t="n"/>
       <c r="L5" s="4" t="n"/>
       <c r="M5" s="3" t="n"/>
     </row>
@@ -2738,7 +3090,7 @@
         </is>
       </c>
       <c r="J6" s="5" t="n"/>
-      <c r="K6" s="3" t="n"/>
+      <c r="K6" s="4" t="n"/>
       <c r="L6" s="4" t="n"/>
       <c r="M6" s="3" t="n"/>
     </row>
@@ -2777,7 +3129,7 @@
         </is>
       </c>
       <c r="J7" s="5" t="n"/>
-      <c r="K7" s="3" t="n"/>
+      <c r="K7" s="4" t="n"/>
       <c r="L7" s="4" t="n"/>
       <c r="M7" s="3" t="n"/>
     </row>
@@ -2785,7 +3137,7 @@
       <c r="A8" s="3" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>MLH-00010</t>
+          <t>HLD-22490</t>
         </is>
       </c>
       <c r="C8" s="4" t="n">
@@ -2814,7 +3166,7 @@
         </is>
       </c>
       <c r="J8" s="5" t="n"/>
-      <c r="K8" s="3" t="n"/>
+      <c r="K8" s="4" t="n"/>
       <c r="L8" s="4" t="n"/>
       <c r="M8" s="3" t="n"/>
     </row>
@@ -2841,6 +3193,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -2942,7 +3295,7 @@
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
     </row>
@@ -2983,7 +3336,7 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K3" s="3" t="n"/>
+      <c r="K3" s="4" t="n"/>
       <c r="L3" s="4" t="n"/>
       <c r="M3" s="3" t="n"/>
     </row>
@@ -3026,7 +3379,7 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="4" t="n"/>
       <c r="L4" s="4" t="n"/>
       <c r="M4" s="3" t="n"/>
     </row>
@@ -3067,7 +3420,7 @@
           <t>N</t>
         </is>
       </c>
-      <c r="K5" s="3" t="n"/>
+      <c r="K5" s="4" t="n"/>
       <c r="L5" s="4" t="n"/>
       <c r="M5" s="3" t="n"/>
     </row>
@@ -3082,7 +3435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3094,6 +3447,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -3195,7 +3549,7 @@
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
     </row>
@@ -3236,7 +3590,7 @@
         </is>
       </c>
       <c r="J3" s="5" t="n"/>
-      <c r="K3" s="3" t="n"/>
+      <c r="K3" s="4" t="n"/>
       <c r="L3" s="4" t="n"/>
       <c r="M3" s="3" t="n"/>
     </row>
@@ -3244,7 +3598,7 @@
       <c r="A4" s="3" t="n"/>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>HLD-22511</t>
+          <t>CLN-00030</t>
         </is>
       </c>
       <c r="C4" s="4" t="n">
@@ -3275,7 +3629,7 @@
         </is>
       </c>
       <c r="J4" s="5" t="n"/>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="4" t="n"/>
       <c r="L4" s="4" t="n"/>
       <c r="M4" s="3" t="n"/>
     </row>
@@ -3283,66 +3637,66 @@
       <c r="A5" s="3" t="n"/>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>MLS-00040</t>
+          <t>CLN-00100</t>
         </is>
       </c>
       <c r="C5" s="4" t="n">
         <v>44629</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>44633</v>
+        <v>44629</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>Hold - Renter</t>
+          <t>Hold - Clean</t>
         </is>
       </c>
       <c r="G5" s="3" t="n"/>
       <c r="H5" s="5" t="inlineStr">
         <is>
+          <t>MS-Add</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
           <t>MS</t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
       <c r="J5" s="5" t="n"/>
-      <c r="K5" s="3" t="n"/>
-      <c r="L5" s="4" t="n">
-        <v>44593</v>
-      </c>
+      <c r="K5" s="4" t="n"/>
+      <c r="L5" s="4" t="n"/>
       <c r="M5" s="3" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="n"/>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>CLN-00060</t>
+          <t>MLS-00020</t>
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>44634</v>
+        <v>44630</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>44634</v>
+        <v>44633</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>Hold - Clean</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>5175</v>
+      </c>
       <c r="H6" s="5" t="inlineStr">
         <is>
-          <t>MS-Add</t>
+          <t>Airbnb</t>
         </is>
       </c>
       <c r="I6" s="5" t="inlineStr">
@@ -3351,7 +3705,7 @@
         </is>
       </c>
       <c r="J6" s="5" t="n"/>
-      <c r="K6" s="3" t="n"/>
+      <c r="K6" s="4" t="n"/>
       <c r="L6" s="4" t="n"/>
       <c r="M6" s="3" t="n"/>
     </row>
@@ -3359,17 +3713,19 @@
       <c r="A7" s="3" t="n"/>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>CLN-00070</t>
+          <t>CLN-00040</t>
         </is>
       </c>
       <c r="C7" s="4" t="n">
-        <v>44643</v>
+        <v>44634</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>44643</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>1</v>
+        <v>44634</v>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
@@ -3379,16 +3735,16 @@
       <c r="G7" s="3" t="n"/>
       <c r="H7" s="5" t="inlineStr">
         <is>
-          <t>MS-Add</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="J7" s="5" t="n"/>
-      <c r="K7" s="3" t="n"/>
+      <c r="K7" s="4" t="n"/>
       <c r="L7" s="4" t="n"/>
       <c r="M7" s="3" t="n"/>
     </row>
@@ -3396,29 +3752,27 @@
       <c r="A8" s="3" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>MLS-00050</t>
+          <t>CLN-00110</t>
         </is>
       </c>
       <c r="C8" s="4" t="n">
-        <v>44644</v>
+        <v>44643</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>44647</v>
+        <v>44643</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>5684.28</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="n"/>
       <c r="H8" s="5" t="inlineStr">
         <is>
-          <t>Airbnb</t>
+          <t>MS-Add</t>
         </is>
       </c>
       <c r="I8" s="5" t="inlineStr">
@@ -3427,7 +3781,7 @@
         </is>
       </c>
       <c r="J8" s="5" t="n"/>
-      <c r="K8" s="3" t="n"/>
+      <c r="K8" s="4" t="n"/>
       <c r="L8" s="4" t="n"/>
       <c r="M8" s="3" t="n"/>
     </row>
@@ -3435,36 +3789,38 @@
       <c r="A9" s="3" t="n"/>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>OWN-00010</t>
+          <t>MLS-00030</t>
         </is>
       </c>
       <c r="C9" s="4" t="n">
+        <v>44644</v>
+      </c>
+      <c r="D9" s="4" t="n">
         <v>44647</v>
       </c>
-      <c r="D9" s="4" t="n">
-        <v>44649</v>
-      </c>
       <c r="E9" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
-          <t>Res.-Owner</t>
-        </is>
-      </c>
-      <c r="G9" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>5684.28</v>
+      </c>
       <c r="H9" s="5" t="inlineStr">
         <is>
+          <t>Airbnb</t>
+        </is>
+      </c>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
           <t>MS</t>
         </is>
       </c>
-      <c r="I9" s="5" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
       <c r="J9" s="5" t="n"/>
-      <c r="K9" s="3" t="n"/>
+      <c r="K9" s="4" t="n"/>
       <c r="L9" s="4" t="n"/>
       <c r="M9" s="3" t="n"/>
     </row>
@@ -3472,14 +3828,14 @@
       <c r="A10" s="3" t="n"/>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>CLN-00080</t>
+          <t>CLN-00050</t>
         </is>
       </c>
       <c r="C10" s="4" t="n">
-        <v>44650</v>
+        <v>44647</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>44650</v>
+        <v>44647</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>1</v>
@@ -3492,7 +3848,7 @@
       <c r="G10" s="3" t="n"/>
       <c r="H10" s="5" t="inlineStr">
         <is>
-          <t>MS-Add</t>
+          <t>Marthas</t>
         </is>
       </c>
       <c r="I10" s="5" t="inlineStr">
@@ -3501,9 +3857,83 @@
         </is>
       </c>
       <c r="J10" s="5" t="n"/>
-      <c r="K10" s="3" t="n"/>
+      <c r="K10" s="4" t="n"/>
       <c r="L10" s="4" t="n"/>
       <c r="M10" s="3" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n"/>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>OWN-00010</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>44647</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44649</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>Res.-Owner</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="n"/>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="I11" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="n"/>
+      <c r="K11" s="4" t="n"/>
+      <c r="L11" s="4" t="n"/>
+      <c r="M11" s="3" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n"/>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>CLN-00060</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>44650</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44650</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="n"/>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>Marthas</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J12" s="5" t="n"/>
+      <c r="K12" s="4" t="n"/>
+      <c r="L12" s="4" t="n"/>
+      <c r="M12" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -3528,6 +3958,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -3629,7 +4060,7 @@
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
     </row>
@@ -3670,7 +4101,7 @@
         </is>
       </c>
       <c r="J3" s="5" t="n"/>
-      <c r="K3" s="3" t="n"/>
+      <c r="K3" s="4" t="n"/>
       <c r="L3" s="4" t="n"/>
       <c r="M3" s="3" t="n"/>
     </row>
@@ -3709,7 +4140,7 @@
         </is>
       </c>
       <c r="J4" s="5" t="n"/>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="4" t="n"/>
       <c r="L4" s="4" t="n"/>
       <c r="M4" s="3" t="n"/>
     </row>
@@ -3748,7 +4179,7 @@
         </is>
       </c>
       <c r="J5" s="5" t="n"/>
-      <c r="K5" s="3" t="n"/>
+      <c r="K5" s="4" t="n"/>
       <c r="L5" s="4" t="n"/>
       <c r="M5" s="3" t="n"/>
     </row>
@@ -3789,7 +4220,7 @@
         </is>
       </c>
       <c r="J6" s="5" t="n"/>
-      <c r="K6" s="3" t="n"/>
+      <c r="K6" s="4" t="n"/>
       <c r="L6" s="4" t="n"/>
       <c r="M6" s="3" t="n"/>
     </row>
@@ -3828,7 +4259,7 @@
         </is>
       </c>
       <c r="J7" s="5" t="n"/>
-      <c r="K7" s="3" t="n"/>
+      <c r="K7" s="4" t="n"/>
       <c r="L7" s="4" t="n"/>
       <c r="M7" s="3" t="n"/>
     </row>
@@ -3867,7 +4298,7 @@
         </is>
       </c>
       <c r="J8" s="5" t="n"/>
-      <c r="K8" s="3" t="n"/>
+      <c r="K8" s="4" t="n"/>
       <c r="L8" s="4" t="n"/>
       <c r="M8" s="3" t="n"/>
     </row>
@@ -3908,7 +4339,7 @@
         </is>
       </c>
       <c r="J9" s="5" t="n"/>
-      <c r="K9" s="3" t="n"/>
+      <c r="K9" s="4" t="n"/>
       <c r="L9" s="4" t="n"/>
       <c r="M9" s="3" t="n"/>
     </row>
@@ -3923,7 +4354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3935,6 +4366,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -4036,7 +4468,7 @@
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
     </row>
@@ -4075,7 +4507,7 @@
         </is>
       </c>
       <c r="J3" s="5" t="n"/>
-      <c r="K3" s="3" t="n"/>
+      <c r="K3" s="4" t="n"/>
       <c r="L3" s="4" t="n"/>
       <c r="M3" s="3" t="n"/>
     </row>
@@ -4116,7 +4548,7 @@
         </is>
       </c>
       <c r="J4" s="5" t="n"/>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="4" t="n"/>
       <c r="L4" s="4" t="n"/>
       <c r="M4" s="3" t="n"/>
     </row>
@@ -4124,7 +4556,7 @@
       <c r="A5" s="3" t="n"/>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>HLD-22530</t>
+          <t>CLN-00070</t>
         </is>
       </c>
       <c r="C5" s="4" t="n">
@@ -4155,7 +4587,7 @@
         </is>
       </c>
       <c r="J5" s="5" t="n"/>
-      <c r="K5" s="3" t="n"/>
+      <c r="K5" s="4" t="n"/>
       <c r="L5" s="4" t="n"/>
       <c r="M5" s="3" t="n"/>
     </row>
@@ -4163,29 +4595,27 @@
       <c r="A6" s="3" t="n"/>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>MLS-00030</t>
+          <t>CLN-00120</t>
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>44700</v>
+        <v>44699</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>44705</v>
+        <v>44699</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="n">
-        <v>11678.8</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="n"/>
       <c r="H6" s="5" t="inlineStr">
         <is>
-          <t>AirBnb</t>
+          <t>MS-Add</t>
         </is>
       </c>
       <c r="I6" s="5" t="inlineStr">
@@ -4194,7 +4624,7 @@
         </is>
       </c>
       <c r="J6" s="5" t="n"/>
-      <c r="K6" s="3" t="n"/>
+      <c r="K6" s="4" t="n"/>
       <c r="L6" s="4" t="n"/>
       <c r="M6" s="3" t="n"/>
     </row>
@@ -4202,36 +4632,38 @@
       <c r="A7" s="3" t="n"/>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>CLN-00030</t>
+          <t>MLS-00040</t>
         </is>
       </c>
       <c r="C7" s="4" t="n">
-        <v>44706</v>
+        <v>44700</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>44706</v>
+        <v>44705</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>Hold - Clean</t>
-        </is>
-      </c>
-      <c r="G7" s="3" t="n"/>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>11678.8</v>
+      </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
+          <t>AirBnb</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
           <t>MS</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
       <c r="J7" s="5" t="n"/>
-      <c r="K7" s="3" t="n"/>
+      <c r="K7" s="4" t="n"/>
       <c r="L7" s="4" t="n"/>
       <c r="M7" s="3" t="n"/>
     </row>
@@ -4239,29 +4671,27 @@
       <c r="A8" s="3" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>MLS-00020</t>
+          <t>CLN-00080</t>
         </is>
       </c>
       <c r="C8" s="4" t="n">
-        <v>44707</v>
+        <v>44706</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>44712</v>
+        <v>44706</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
-          <t>Res. - Renter</t>
-        </is>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>5881</v>
-      </c>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="n"/>
       <c r="H8" s="5" t="inlineStr">
         <is>
-          <t>AirBnb</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="I8" s="5" t="inlineStr">
@@ -4270,9 +4700,48 @@
         </is>
       </c>
       <c r="J8" s="5" t="n"/>
-      <c r="K8" s="3" t="n"/>
+      <c r="K8" s="4" t="n"/>
       <c r="L8" s="4" t="n"/>
       <c r="M8" s="3" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n"/>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>MLS-00050</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>44707</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44712</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>Res. - Renter</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>5881</v>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t>AirBnb</t>
+        </is>
+      </c>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J9" s="5" t="n"/>
+      <c r="K9" s="4" t="n"/>
+      <c r="L9" s="4" t="n"/>
+      <c r="M9" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -4285,7 +4754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4297,6 +4766,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -4367,7 +4837,7 @@
       <c r="A2" s="3" t="n"/>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>MLS-00060</t>
+          <t>HLD-22839</t>
         </is>
       </c>
       <c r="C2" s="4" t="n">
@@ -4383,24 +4853,61 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>Hold - Renter</t>
+          <t>Hold - Owner</t>
         </is>
       </c>
       <c r="G2" s="3" t="n"/>
       <c r="H2" s="5" t="inlineStr">
         <is>
-          <t>WineClub</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="I2" s="5" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>BP</t>
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>CLN-00090</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>44713</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44713</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Hold - Clean</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="n"/>
+      <c r="K3" s="4" t="n"/>
+      <c r="L3" s="4" t="n"/>
+      <c r="M3" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -4413,7 +4920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4425,6 +4932,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -4490,43 +4998,6 @@
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n"/>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>CLN-00040</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="n">
-        <v>44743</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>44743</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>Hold - Clean</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="n"/>
-      <c r="H2" s="5" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
-      <c r="I2" s="5" t="inlineStr">
-        <is>
-          <t>MS</t>
-        </is>
-      </c>
-      <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
-      <c r="L2" s="4" t="n"/>
-      <c r="M2" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -4551,6 +5022,7 @@
     <col customWidth="1" max="3" min="3" width="12"/>
     <col customWidth="1" max="4" min="4" width="12"/>
     <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
     <col customWidth="1" max="8" min="8" width="17"/>
     <col customWidth="1" max="9" min="9" width="15"/>
     <col customWidth="1" max="10" min="10" width="12"/>
@@ -4652,7 +5124,7 @@
         </is>
       </c>
       <c r="J2" s="5" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="4" t="n"/>
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="3" t="n"/>
     </row>

</xml_diff>